<commit_message>
Minor tweaks to log messages and comments
</commit_message>
<xml_diff>
--- a/tests/samples/admin_umag.xlsx
+++ b/tests/samples/admin_umag.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\r.hawke\PycharmProjects\Mass-Circular-Weighing\tests\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C758B26B-2EBD-4C1E-ABFE-5FFE8CF6E835}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F445AFE2-550B-46F9-997B-54BC0B27EC2B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25590" yWindow="2070" windowWidth="21780" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Admin" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="116">
   <si>
     <t>Title</t>
   </si>
@@ -376,6 +376,12 @@
   </si>
   <si>
     <t>95% CI (mg)</t>
+  </si>
+  <si>
+    <t>CI in mass histories</t>
+  </si>
+  <si>
+    <t>diff</t>
   </si>
 </sst>
 </file>
@@ -385,8 +391,8 @@
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.000\ 000\ 000"/>
-    <numFmt numFmtId="170" formatCode="0.000000000"/>
-    <numFmt numFmtId="175" formatCode="0.000\ 0"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
+    <numFmt numFmtId="167" formatCode="0.000\ 0"/>
   </numFmts>
   <fonts count="8" x14ac:knownFonts="1">
     <font>
@@ -555,7 +561,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -650,43 +656,44 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="175" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1003,8 +1010,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15:E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1023,17 +1030,17 @@
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="50" t="s">
         <v>75</v>
       </c>
-      <c r="C1" s="46"/>
+      <c r="C1" s="51"/>
       <c r="D1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="45" t="s">
+      <c r="E1" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="52"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="10" t="s">
@@ -1060,9 +1067,9 @@
       <c r="D3" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="E3" s="49"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
+      <c r="E3" s="54"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
     </row>
     <row r="4" spans="1:8" s="10" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="10" t="s">
@@ -1103,41 +1110,41 @@
       <c r="A7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="44" t="s">
+      <c r="B7" s="49" t="s">
         <v>44</v>
       </c>
-      <c r="C7" s="43"/>
+      <c r="C7" s="48"/>
       <c r="D7" s="4" t="s">
         <v>15</v>
       </c>
       <c r="E7" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="F7" s="42" t="s">
+      <c r="F7" s="47" t="s">
         <v>16</v>
       </c>
-      <c r="G7" s="43"/>
-      <c r="H7" s="43"/>
+      <c r="G7" s="48"/>
+      <c r="H7" s="48"/>
     </row>
     <row r="8" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="44" t="s">
+      <c r="B8" s="49" t="s">
         <v>58</v>
       </c>
-      <c r="C8" s="43"/>
+      <c r="C8" s="48"/>
       <c r="D8" s="4" t="s">
         <v>18</v>
       </c>
       <c r="E8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="F8" s="42" t="s">
+      <c r="F8" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="G8" s="43"/>
-      <c r="H8" s="43"/>
+      <c r="G8" s="48"/>
+      <c r="H8" s="48"/>
     </row>
     <row r="9" spans="1:8" s="2" customFormat="1" ht="35" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="5" t="s">
@@ -1153,11 +1160,11 @@
         <v>21</v>
       </c>
       <c r="E9" s="19"/>
-      <c r="F9" s="42" t="s">
+      <c r="F9" s="47" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
+      <c r="G9" s="48"/>
+      <c r="H9" s="48"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
@@ -1181,10 +1188,10 @@
       <c r="D11" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E11" s="51" t="s">
+      <c r="E11" s="56" t="s">
         <v>87</v>
       </c>
-      <c r="F11" s="52"/>
+      <c r="F11" s="57"/>
       <c r="G11" s="14" t="s">
         <v>26</v>
       </c>
@@ -1197,8 +1204,8 @@
       <c r="A13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="B13" s="47"/>
-      <c r="C13" s="48"/>
+      <c r="B13" s="52"/>
+      <c r="C13" s="53"/>
       <c r="F13" s="14"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1853,7 +1860,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:K16"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1882,7 +1889,7 @@
       <c r="E1" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="54"/>
+      <c r="F1" s="44"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="29" t="s">
@@ -1900,8 +1907,8 @@
       <c r="E2" s="35">
         <v>0</v>
       </c>
-      <c r="F2" s="55"/>
-      <c r="N2" s="53"/>
+      <c r="F2" s="45"/>
+      <c r="N2" s="43"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="33" t="s">
@@ -1919,8 +1926,8 @@
       <c r="E3" s="35">
         <v>-1.9910000000000001</v>
       </c>
-      <c r="F3" s="55"/>
-      <c r="N3" s="53"/>
+      <c r="F3" s="45"/>
+      <c r="N3" s="43"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="38" t="s">
@@ -1938,8 +1945,8 @@
       <c r="E4" s="35">
         <v>-1.9910000000000001</v>
       </c>
-      <c r="F4" s="55"/>
-      <c r="N4" s="53"/>
+      <c r="F4" s="45"/>
+      <c r="N4" s="43"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="33" t="s">
@@ -1957,8 +1964,8 @@
       <c r="E5" s="35">
         <v>0</v>
       </c>
-      <c r="F5" s="55"/>
-      <c r="N5" s="53"/>
+      <c r="F5" s="45"/>
+      <c r="N5" s="43"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="33" t="s">
@@ -1976,8 +1983,8 @@
       <c r="E6" s="35">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="F6" s="55"/>
-      <c r="N6" s="53"/>
+      <c r="F6" s="45"/>
+      <c r="N6" s="43"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="33" t="s">
@@ -1995,8 +2002,8 @@
       <c r="E7" s="35">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="F7" s="55"/>
-      <c r="N7" s="53"/>
+      <c r="F7" s="45"/>
+      <c r="N7" s="43"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="29" t="s">
@@ -2014,8 +2021,8 @@
       <c r="E8" s="35">
         <v>0</v>
       </c>
-      <c r="F8" s="55"/>
-      <c r="N8" s="53"/>
+      <c r="F8" s="45"/>
+      <c r="N8" s="43"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="33" t="s">
@@ -2033,8 +2040,8 @@
       <c r="E9" s="35">
         <v>-5.5190000000000001</v>
       </c>
-      <c r="F9" s="55"/>
-      <c r="N9" s="53"/>
+      <c r="F9" s="45"/>
+      <c r="N9" s="43"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="38" t="s">
@@ -2052,8 +2059,8 @@
       <c r="E10" s="35">
         <v>-5.5190000000000001</v>
       </c>
-      <c r="F10" s="55"/>
-      <c r="N10" s="53"/>
+      <c r="F10" s="45"/>
+      <c r="N10" s="43"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="33" t="s">
@@ -2071,8 +2078,8 @@
       <c r="E11" s="35">
         <v>0</v>
       </c>
-      <c r="F11" s="55"/>
-      <c r="N11" s="53"/>
+      <c r="F11" s="45"/>
+      <c r="N11" s="43"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="33" t="s">
@@ -2090,8 +2097,8 @@
       <c r="E12" s="35">
         <v>4.7629999999999999</v>
       </c>
-      <c r="F12" s="55"/>
-      <c r="N12" s="53"/>
+      <c r="F12" s="45"/>
+      <c r="N12" s="43"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="33" t="s">
@@ -2109,8 +2116,8 @@
       <c r="E13" s="35">
         <v>4.7629999999999999</v>
       </c>
-      <c r="F13" s="55"/>
-      <c r="N13" s="53"/>
+      <c r="F13" s="45"/>
+      <c r="N13" s="43"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="29" t="s">
@@ -2128,8 +2135,8 @@
       <c r="E14" s="35">
         <v>0</v>
       </c>
-      <c r="F14" s="55"/>
-      <c r="N14" s="53"/>
+      <c r="F14" s="45"/>
+      <c r="N14" s="43"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="33" t="s">
@@ -2147,8 +2154,8 @@
       <c r="E15" s="35">
         <v>2.7029999999999998</v>
       </c>
-      <c r="F15" s="55"/>
-      <c r="N15" s="53"/>
+      <c r="F15" s="45"/>
+      <c r="N15" s="43"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" s="38" t="s">
@@ -2166,15 +2173,15 @@
       <c r="E16" s="35">
         <v>2.7029999999999998</v>
       </c>
-      <c r="F16" s="55"/>
-      <c r="N16" s="53"/>
+      <c r="F16" s="45"/>
+      <c r="N16" s="43"/>
     </row>
     <row r="17" spans="5:6" x14ac:dyDescent="0.35">
       <c r="E17" s="35"/>
-      <c r="F17" s="55"/>
+      <c r="F17" s="45"/>
     </row>
     <row r="18" spans="5:6" x14ac:dyDescent="0.35">
-      <c r="F18" s="54"/>
+      <c r="F18" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2183,10 +2190,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3D148F2-7C3F-4D51-BA01-6094ADD4F25D}">
-  <dimension ref="A1:K14"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P14" sqref="P14:P23"/>
+      <selection activeCell="N8" sqref="N8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2196,7 +2203,7 @@
     <col min="7" max="7" width="9.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="35" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" s="35" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="35" t="s">
         <v>102</v>
       </c>
@@ -2224,9 +2231,15 @@
       <c r="K1" s="35" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A2" s="55"/>
+      <c r="L1" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="M1" s="35" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="45"/>
       <c r="B2">
         <v>10000</v>
       </c>
@@ -2236,7 +2249,7 @@
       <c r="D2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="56">
+      <c r="E2" s="46">
         <v>10000.085866240001</v>
       </c>
       <c r="F2">
@@ -2252,9 +2265,16 @@
         <f>G2/1000</f>
         <v>0.84191300000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A3" s="55"/>
+      <c r="L2" s="42">
+        <v>0.84191399999999994</v>
+      </c>
+      <c r="M2">
+        <f>K2-L2</f>
+        <v>-9.9999999991773336E-7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="45"/>
       <c r="B3">
         <v>10000</v>
       </c>
@@ -2264,7 +2284,7 @@
       <c r="D3" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="56">
+      <c r="E3" s="46">
         <v>10000.044098218001</v>
       </c>
       <c r="F3">
@@ -2280,9 +2300,16 @@
         <f t="shared" ref="K3:K11" si="0">G3/1000</f>
         <v>0.84255400000000003</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A4" s="55"/>
+      <c r="L3" s="42">
+        <v>0.84255400000000003</v>
+      </c>
+      <c r="M3" s="42">
+        <f t="shared" ref="M3:M11" si="1">K3-L3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="45"/>
       <c r="B4">
         <v>10000</v>
       </c>
@@ -2292,7 +2319,7 @@
       <c r="D4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="56">
+      <c r="E4" s="46">
         <v>10000.015992981</v>
       </c>
       <c r="F4">
@@ -2308,9 +2335,16 @@
         <f t="shared" si="0"/>
         <v>0.85037400000000007</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A5" s="55"/>
+      <c r="L4" s="42">
+        <v>0.85037368837708471</v>
+      </c>
+      <c r="M4" s="42">
+        <f t="shared" si="1"/>
+        <v>3.116229153610206E-7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="45"/>
       <c r="B5">
         <v>10000</v>
       </c>
@@ -2320,7 +2354,7 @@
       <c r="D5" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="56">
+      <c r="E5" s="46">
         <v>10000.150514306</v>
       </c>
       <c r="F5">
@@ -2336,9 +2370,16 @@
         <f t="shared" si="0"/>
         <v>64.186025999999998</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A6" s="55"/>
+      <c r="L5" s="42">
+        <v>64.18602605707224</v>
+      </c>
+      <c r="M5" s="42">
+        <f t="shared" si="1"/>
+        <v>-5.7072242043432198E-8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="45"/>
       <c r="B6">
         <v>10000</v>
       </c>
@@ -2348,7 +2389,7 @@
       <c r="D6" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="56">
+      <c r="E6" s="46">
         <v>9999.9027681660009</v>
       </c>
       <c r="F6">
@@ -2364,9 +2405,16 @@
         <f t="shared" si="0"/>
         <v>0.84190599999999993</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A7" s="55"/>
+      <c r="L6" s="42">
+        <v>0.84190599999999993</v>
+      </c>
+      <c r="M6" s="42">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="45"/>
       <c r="B7">
         <v>10000</v>
       </c>
@@ -2376,7 +2424,7 @@
       <c r="D7" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="56">
+      <c r="E7" s="46">
         <v>10000.016499648</v>
       </c>
       <c r="F7">
@@ -2392,9 +2440,16 @@
         <f t="shared" si="0"/>
         <v>28.814467</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A8" s="55"/>
+      <c r="L7">
+        <v>28.814466884851551</v>
+      </c>
+      <c r="M7" s="42">
+        <f t="shared" si="1"/>
+        <v>1.1514844899807031E-7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="45"/>
       <c r="B8">
         <v>10000</v>
       </c>
@@ -2404,7 +2459,7 @@
       <c r="D8" t="s">
         <v>5</v>
       </c>
-      <c r="E8" s="56">
+      <c r="E8" s="46">
         <v>9999.9741830179992</v>
       </c>
       <c r="F8">
@@ -2420,9 +2475,16 @@
         <f t="shared" si="0"/>
         <v>0.84190900000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" s="55"/>
+      <c r="L8">
+        <v>0.84190799999999999</v>
+      </c>
+      <c r="M8" s="42">
+        <f t="shared" si="1"/>
+        <v>1.0000000000287557E-6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="45"/>
       <c r="B9">
         <v>10000</v>
       </c>
@@ -2432,7 +2494,7 @@
       <c r="D9" t="s">
         <v>5</v>
       </c>
-      <c r="E9" s="56">
+      <c r="E9" s="46">
         <v>10000.042358572</v>
       </c>
       <c r="F9">
@@ -2448,9 +2510,16 @@
         <f t="shared" si="0"/>
         <v>43.836285000000004</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" s="55"/>
+      <c r="L9">
+        <v>43.836285342311619</v>
+      </c>
+      <c r="M9" s="42">
+        <f t="shared" si="1"/>
+        <v>-3.423116154976924E-7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="45"/>
       <c r="B10">
         <v>10000</v>
       </c>
@@ -2460,7 +2529,7 @@
       <c r="D10" t="s">
         <v>5</v>
       </c>
-      <c r="E10" s="56">
+      <c r="E10" s="46">
         <v>10000.119090796001</v>
       </c>
       <c r="F10">
@@ -2476,9 +2545,16 @@
         <f t="shared" si="0"/>
         <v>20.269239000000002</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" s="55"/>
+      <c r="L10">
+        <v>20.26923914929991</v>
+      </c>
+      <c r="M10" s="42">
+        <f t="shared" si="1"/>
+        <v>-1.4929990754808387E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="45"/>
       <c r="B11">
         <v>10000</v>
       </c>
@@ -2488,7 +2564,7 @@
       <c r="D11" t="s">
         <v>5</v>
       </c>
-      <c r="E11" s="56">
+      <c r="E11" s="46">
         <v>10000.038388898</v>
       </c>
       <c r="F11">
@@ -2504,9 +2580,16 @@
         <f t="shared" si="0"/>
         <v>20.842508000000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" s="55"/>
+      <c r="L11">
+        <v>20.842508177843392</v>
+      </c>
+      <c r="M11" s="42">
+        <f t="shared" si="1"/>
+        <v>-1.7784338979254244E-7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="45"/>
       <c r="B12">
         <v>10000</v>
       </c>
@@ -2516,7 +2599,7 @@
       <c r="D12" t="s">
         <v>24</v>
       </c>
-      <c r="E12" s="56">
+      <c r="E12" s="46">
         <v>10000.00499293</v>
       </c>
       <c r="F12">
@@ -2534,9 +2617,10 @@
       <c r="J12" s="35" t="s">
         <v>98</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" s="55"/>
+      <c r="M12" s="42"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A13" s="45"/>
       <c r="B13">
         <v>10000</v>
       </c>
@@ -2546,7 +2630,7 @@
       <c r="D13" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="56">
+      <c r="E13" s="46">
         <v>10000.003261551001</v>
       </c>
       <c r="F13">
@@ -2564,9 +2648,10 @@
       <c r="J13" s="35" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" s="54"/>
+      <c r="M13" s="42"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A14" s="44"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>